<commit_message>
Print set to own bin
</commit_message>
<xml_diff>
--- a/bin/print/BillingReport.xlsx
+++ b/bin/print/BillingReport.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICS\bin\print\ori\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$N$357</definedName>
+    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$N$84</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -23,9 +18,10 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Daily_Report" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" codePage="437" sourceFile="E:\ICS\bin\print\Daily_Report.txt" tab="0" delimiter="|">
-      <textFields count="13">
+  <connection id="1" name="Daily_Report" type="6" refreshedVersion="3" background="1" refreshOnLoad="1">
+    <textPr prompt="0" codePage="437" sourceFile="E:\ICS_Udugama\bin\print\Daily_Report.txt" tab="0" delimiter="|">
+      <textFields count="14">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -46,22 +42,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,7 +252,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Daily_Report1" refreshOnLoad="1" growShrinkType="overwriteClear" fillFormulas="1" adjustColumnWidth="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Daily_Report1" refreshOnLoad="1" growShrinkType="overwriteClear" fillFormulas="1" removeDataOnSave="1" adjustColumnWidth="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -309,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,10 +330,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,7 +364,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -552,30 +539,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M357"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O357"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
-    <col min="5" max="9" width="8.7109375" style="7" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="8.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" style="7" customWidth="1"/>
+    <col min="8" max="10" width="7.5703125" style="7" customWidth="1"/>
+    <col min="11" max="14" width="10.28515625" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="10"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -584,8 +573,10 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="10"/>
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -599,1113 +590,2122 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="6"/>
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="O45"/>
+    </row>
+    <row r="46" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
       <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
       <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
       <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
       <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
       <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
       <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
       <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
       <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
       <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="O63"/>
+    </row>
+    <row r="64" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
       <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="O68"/>
+    </row>
+    <row r="69" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="O69"/>
+    </row>
+    <row r="70" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
       <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="5"/>
-    </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="5"/>
-    </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="O73"/>
+    </row>
+    <row r="74" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="5"/>
-    </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="O74"/>
+    </row>
+    <row r="75" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
       <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
       <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="O76"/>
+    </row>
+    <row r="77" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="O77"/>
+    </row>
+    <row r="78" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
       <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="O78"/>
+    </row>
+    <row r="79" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
       <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+      <c r="O79"/>
+    </row>
+    <row r="80" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
       <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="O80"/>
+    </row>
+    <row r="81" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
       <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="O81"/>
+    </row>
+    <row r="82" spans="1:15" ht="14.25" customHeight="1">
       <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="1:15" ht="14.25" customHeight="1">
       <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="1:15" ht="14.25" customHeight="1">
       <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D84" s="4"/>
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="1:15" ht="14.25" customHeight="1">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="14.25" customHeight="1">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="14.25" customHeight="1">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="14.25" customHeight="1">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="14.25" customHeight="1">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="14.25" customHeight="1">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="14.25" customHeight="1">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="14.25" customHeight="1">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="14.25" customHeight="1">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="14.25" customHeight="1">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="14.25" customHeight="1">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" ht="14.25" customHeight="1">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:3" ht="14.25" customHeight="1">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:3" ht="14.25" customHeight="1">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:3" ht="14.25" customHeight="1">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:3" ht="14.25" customHeight="1">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:3" ht="14.25" customHeight="1">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:3" ht="14.25" customHeight="1">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:3" ht="14.25" customHeight="1">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:3" ht="14.25" customHeight="1">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:3" ht="14.25" customHeight="1">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:3" ht="14.25" customHeight="1">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:3" ht="14.25" customHeight="1">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:3" ht="14.25" customHeight="1">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:3" ht="14.25" customHeight="1">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:3" ht="14.25" customHeight="1">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:3" ht="14.25" customHeight="1">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:3" ht="14.25" customHeight="1">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:3" ht="14.25" customHeight="1">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:3" ht="14.25" customHeight="1">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:3" ht="14.25" customHeight="1">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:3" ht="14.25" customHeight="1">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:3" ht="14.25" customHeight="1">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:3" ht="14.25" customHeight="1">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:3" ht="14.25" customHeight="1">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:3" ht="14.25" customHeight="1">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:3" ht="14.25" customHeight="1">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:3" ht="14.25" customHeight="1">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:3" ht="14.25" customHeight="1">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:3" ht="14.25" customHeight="1">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:3" ht="14.25" customHeight="1">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:3" ht="14.25" customHeight="1">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:3" ht="14.25" customHeight="1">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:3" ht="14.25" customHeight="1">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:3" ht="14.25" customHeight="1">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:3" ht="14.25" customHeight="1">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:3" ht="14.25" customHeight="1">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:3" ht="14.25" customHeight="1">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:3" ht="14.25" customHeight="1">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:3" ht="14.25" customHeight="1">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:3" ht="14.25" customHeight="1">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:3" ht="14.25" customHeight="1">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:3" ht="14.25" customHeight="1">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:3" ht="14.25" customHeight="1">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:3" ht="14.25" customHeight="1">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:3" ht="14.25" customHeight="1">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:3" ht="14.25" customHeight="1">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:3" ht="14.25" customHeight="1">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:3" ht="14.25" customHeight="1">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:3" ht="14.25" customHeight="1">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:3" ht="14.25" customHeight="1">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:3" ht="14.25" customHeight="1">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:3" ht="14.25" customHeight="1">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:3" ht="14.25" customHeight="1">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:3" ht="14.25" customHeight="1">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:3" ht="14.25" customHeight="1">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:3" ht="14.25" customHeight="1">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:3" ht="14.25" customHeight="1">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:3" ht="14.25" customHeight="1">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:3" ht="14.25" customHeight="1">
       <c r="C154" s="5"/>
     </row>
-    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:3" ht="14.25" customHeight="1">
       <c r="C155" s="5"/>
     </row>
-    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:3" ht="14.25" customHeight="1">
       <c r="C156" s="5"/>
     </row>
-    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:3" ht="14.25" customHeight="1">
       <c r="C157" s="5"/>
     </row>
-    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:3" ht="14.25" customHeight="1">
       <c r="C158" s="5"/>
     </row>
-    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:3" ht="14.25" customHeight="1">
       <c r="C159" s="5"/>
     </row>
-    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:3" ht="14.25" customHeight="1">
       <c r="C160" s="5"/>
     </row>
-    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:3" ht="14.25" customHeight="1">
       <c r="C161" s="5"/>
     </row>
-    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:3" ht="14.25" customHeight="1">
       <c r="C162" s="5"/>
     </row>
-    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:3" ht="14.25" customHeight="1">
       <c r="C163" s="5"/>
     </row>
-    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:3" ht="14.25" customHeight="1">
       <c r="C164" s="5"/>
     </row>
-    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:3" ht="14.25" customHeight="1">
       <c r="C165" s="5"/>
     </row>
-    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:3" ht="14.25" customHeight="1">
       <c r="C166" s="5"/>
     </row>
-    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:3" ht="14.25" customHeight="1">
       <c r="C167" s="5"/>
     </row>
-    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:3" ht="14.25" customHeight="1">
       <c r="C168" s="5"/>
     </row>
-    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:3" ht="14.25" customHeight="1">
       <c r="C169" s="5"/>
     </row>
-    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:3" ht="14.25" customHeight="1">
       <c r="C170" s="5"/>
     </row>
-    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:3" ht="14.25" customHeight="1">
       <c r="C171" s="5"/>
     </row>
-    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:3" ht="14.25" customHeight="1">
       <c r="C172" s="5"/>
     </row>
-    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:3" ht="14.25" customHeight="1">
       <c r="C173" s="5"/>
     </row>
-    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:3" ht="14.25" customHeight="1">
       <c r="C174" s="5"/>
     </row>
-    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:3" ht="14.25" customHeight="1">
       <c r="C175" s="5"/>
     </row>
-    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:3" ht="14.25" customHeight="1">
       <c r="C176" s="5"/>
     </row>
-    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:3" ht="14.25" customHeight="1">
       <c r="C177" s="5"/>
     </row>
-    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:3" ht="14.25" customHeight="1">
       <c r="C178" s="5"/>
     </row>
-    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:3" ht="14.25" customHeight="1">
       <c r="C179" s="5"/>
     </row>
-    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:3" ht="14.25" customHeight="1">
       <c r="C180" s="5"/>
     </row>
-    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:3" ht="14.25" customHeight="1">
       <c r="C181" s="5"/>
     </row>
-    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:3" ht="14.25" customHeight="1">
       <c r="C182" s="5"/>
     </row>
-    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:3" ht="14.25" customHeight="1">
       <c r="C183" s="5"/>
     </row>
-    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:3" ht="14.25" customHeight="1">
       <c r="C184" s="5"/>
     </row>
-    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:3" ht="14.25" customHeight="1">
       <c r="C185" s="5"/>
     </row>
-    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:3" ht="14.25" customHeight="1">
       <c r="C186" s="5"/>
     </row>
-    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:3" ht="14.25" customHeight="1">
       <c r="C187" s="5"/>
     </row>
-    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:3" ht="14.25" customHeight="1">
       <c r="C188" s="5"/>
     </row>
-    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:3" ht="14.25" customHeight="1">
       <c r="C189" s="5"/>
     </row>
-    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:3" ht="14.25" customHeight="1">
       <c r="C190" s="5"/>
     </row>
-    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:3" ht="14.25" customHeight="1">
       <c r="C191" s="5"/>
     </row>
-    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:3" ht="14.25" customHeight="1">
       <c r="C192" s="5"/>
     </row>
-    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:3" ht="14.25" customHeight="1">
       <c r="C193" s="5"/>
     </row>
-    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:3" ht="14.25" customHeight="1">
       <c r="C194" s="5"/>
     </row>
-    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:3" ht="14.25" customHeight="1">
       <c r="C195" s="5"/>
     </row>
-    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:3" ht="14.25" customHeight="1">
       <c r="C196" s="5"/>
     </row>
-    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:3" ht="14.25" customHeight="1">
       <c r="C197" s="5"/>
     </row>
-    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:3" ht="14.25" customHeight="1">
       <c r="C198" s="5"/>
     </row>
-    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:3" ht="14.25" customHeight="1">
       <c r="C199" s="5"/>
     </row>
-    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:3" ht="14.25" customHeight="1">
       <c r="C200" s="5"/>
     </row>
-    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:3" ht="14.25" customHeight="1">
       <c r="C201" s="5"/>
     </row>
-    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:3" ht="14.25" customHeight="1">
       <c r="C202" s="5"/>
     </row>
-    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:3" ht="14.25" customHeight="1">
       <c r="C203" s="5"/>
     </row>
-    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:3" ht="14.25" customHeight="1">
       <c r="C204" s="5"/>
     </row>
-    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:3" ht="14.25" customHeight="1">
       <c r="C205" s="5"/>
     </row>
-    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:3" ht="14.25" customHeight="1">
       <c r="C206" s="5"/>
     </row>
-    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:3" ht="14.25" customHeight="1">
       <c r="C207" s="5"/>
     </row>
-    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:3" ht="14.25" customHeight="1">
       <c r="C208" s="5"/>
     </row>
-    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:3" ht="14.25" customHeight="1">
       <c r="C209" s="5"/>
     </row>
-    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:3" ht="14.25" customHeight="1">
       <c r="C210" s="5"/>
     </row>
-    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:3" ht="14.25" customHeight="1">
       <c r="C211" s="5"/>
     </row>
-    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:3" ht="14.25" customHeight="1">
       <c r="C212" s="5"/>
     </row>
-    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:3" ht="14.25" customHeight="1">
       <c r="C213" s="5"/>
     </row>
-    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:3" ht="14.25" customHeight="1">
       <c r="C214" s="5"/>
     </row>
-    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:3" ht="14.25" customHeight="1">
       <c r="C215" s="5"/>
     </row>
-    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:3" ht="14.25" customHeight="1">
       <c r="C216" s="5"/>
     </row>
-    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:3" ht="14.25" customHeight="1">
       <c r="C217" s="5"/>
     </row>
-    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:3" ht="14.25" customHeight="1">
       <c r="C218" s="5"/>
     </row>
-    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:3" ht="14.25" customHeight="1">
       <c r="C219" s="5"/>
     </row>
-    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:3" ht="14.25" customHeight="1">
       <c r="C220" s="5"/>
     </row>
-    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:3" ht="14.25" customHeight="1">
       <c r="C221" s="5"/>
     </row>
-    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:3" ht="14.25" customHeight="1">
       <c r="C222" s="5"/>
     </row>
-    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:3" ht="14.25" customHeight="1">
       <c r="C223" s="5"/>
     </row>
-    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:3" ht="14.25" customHeight="1">
       <c r="C224" s="5"/>
     </row>
-    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:3" ht="14.25" customHeight="1">
       <c r="C225" s="5"/>
     </row>
-    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:3" ht="14.25" customHeight="1">
       <c r="C226" s="5"/>
     </row>
-    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:3" ht="14.25" customHeight="1">
       <c r="C227" s="5"/>
     </row>
-    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:3" ht="14.25" customHeight="1">
       <c r="C228" s="5"/>
     </row>
-    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:3" ht="14.25" customHeight="1">
       <c r="C229" s="5"/>
     </row>
-    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:3" ht="14.25" customHeight="1">
       <c r="C230" s="5"/>
     </row>
-    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:3" ht="14.25" customHeight="1">
       <c r="C231" s="5"/>
     </row>
-    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:3" ht="14.25" customHeight="1">
       <c r="C232" s="5"/>
     </row>
-    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:3" ht="14.25" customHeight="1">
       <c r="C233" s="5"/>
     </row>
-    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:3" ht="14.25" customHeight="1">
       <c r="C234" s="5"/>
     </row>
-    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:3" ht="14.25" customHeight="1">
       <c r="C235" s="5"/>
     </row>
-    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:3" ht="14.25" customHeight="1">
       <c r="C236" s="5"/>
     </row>
-    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:3" ht="14.25" customHeight="1">
       <c r="C237" s="5"/>
     </row>
-    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:3" ht="14.25" customHeight="1">
       <c r="C238" s="5"/>
     </row>
-    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:3" ht="14.25" customHeight="1">
       <c r="C239" s="5"/>
     </row>
-    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:3" ht="14.25" customHeight="1">
       <c r="C240" s="5"/>
     </row>
-    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:3" ht="14.25" customHeight="1">
       <c r="C241" s="5"/>
     </row>
-    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="3:3" ht="14.25" customHeight="1">
       <c r="C242" s="5"/>
     </row>
-    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="3:3" ht="14.25" customHeight="1">
       <c r="C243" s="5"/>
     </row>
-    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="3:3" ht="14.25" customHeight="1">
       <c r="C244" s="5"/>
     </row>
-    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="3:3" ht="14.25" customHeight="1">
       <c r="C245" s="5"/>
     </row>
-    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:3" ht="14.25" customHeight="1">
       <c r="C246" s="5"/>
     </row>
-    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:3" ht="14.25" customHeight="1">
       <c r="C247" s="5"/>
     </row>
-    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:3" ht="14.25" customHeight="1">
       <c r="C248" s="5"/>
     </row>
-    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:3" ht="14.25" customHeight="1">
       <c r="C249" s="5"/>
     </row>
-    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:3" ht="14.25" customHeight="1">
       <c r="C250" s="5"/>
     </row>
-    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:3" ht="14.25" customHeight="1">
       <c r="C251" s="5"/>
     </row>
-    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:3" ht="14.25" customHeight="1">
       <c r="C252" s="5"/>
     </row>
-    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:3" ht="14.25" customHeight="1">
       <c r="C253" s="5"/>
     </row>
-    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="3:3" ht="14.25" customHeight="1">
       <c r="C254" s="5"/>
     </row>
-    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="3:3" ht="14.25" customHeight="1">
       <c r="C255" s="5"/>
     </row>
-    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="3:3" ht="14.25" customHeight="1">
       <c r="C256" s="5"/>
     </row>
-    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:3" ht="14.25" customHeight="1">
       <c r="C257" s="5"/>
     </row>
-    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:3" ht="14.25" customHeight="1">
       <c r="C258" s="5"/>
     </row>
-    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:3" ht="14.25" customHeight="1">
       <c r="C259" s="5"/>
     </row>
-    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:3" ht="14.25" customHeight="1">
       <c r="C260" s="5"/>
     </row>
-    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:3" ht="14.25" customHeight="1">
       <c r="C261" s="5"/>
     </row>
-    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:3" ht="14.25" customHeight="1">
       <c r="C262" s="5"/>
     </row>
-    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:3" ht="14.25" customHeight="1">
       <c r="C263" s="5"/>
     </row>
-    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:3" ht="14.25" customHeight="1">
       <c r="C264" s="5"/>
     </row>
-    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:3" ht="14.25" customHeight="1">
       <c r="C265" s="5"/>
     </row>
-    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:3" ht="14.25" customHeight="1">
       <c r="C266" s="5"/>
     </row>
-    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:3" ht="14.25" customHeight="1">
       <c r="C267" s="5"/>
     </row>
-    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:3" ht="14.25" customHeight="1">
       <c r="C268" s="5"/>
     </row>
-    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="3:3" ht="14.25" customHeight="1">
       <c r="C269" s="5"/>
     </row>
-    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="3:3" ht="14.25" customHeight="1">
       <c r="C270" s="5"/>
     </row>
-    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="3:3" ht="14.25" customHeight="1">
       <c r="C271" s="5"/>
     </row>
-    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="3:3" ht="14.25" customHeight="1">
       <c r="C272" s="5"/>
     </row>
-    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:3" ht="14.25" customHeight="1">
       <c r="C273" s="5"/>
     </row>
-    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:3" ht="14.25" customHeight="1">
       <c r="C274" s="5"/>
     </row>
-    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:3" ht="14.25" customHeight="1">
       <c r="C275" s="5"/>
     </row>
-    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:3" ht="14.25" customHeight="1">
       <c r="C276" s="5"/>
     </row>
-    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:3" ht="14.25" customHeight="1">
       <c r="C277" s="5"/>
     </row>
-    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:3" ht="14.25" customHeight="1">
       <c r="C278" s="5"/>
     </row>
-    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:3" ht="14.25" customHeight="1">
       <c r="C279" s="5"/>
     </row>
-    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:3" ht="14.25" customHeight="1">
       <c r="C280" s="5"/>
     </row>
-    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:3" ht="14.25" customHeight="1">
       <c r="C281" s="5"/>
     </row>
-    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:3" ht="14.25" customHeight="1">
       <c r="C282" s="5"/>
     </row>
-    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:3" ht="14.25" customHeight="1">
       <c r="C283" s="5"/>
     </row>
-    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:3" ht="14.25" customHeight="1">
       <c r="C284" s="5"/>
     </row>
-    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:3" ht="14.25" customHeight="1">
       <c r="C285" s="5"/>
     </row>
-    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:3" ht="14.25" customHeight="1">
       <c r="C286" s="5"/>
     </row>
-    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:3" ht="14.25" customHeight="1">
       <c r="C287" s="5"/>
     </row>
-    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:3" ht="14.25" customHeight="1">
       <c r="C288" s="5"/>
     </row>
-    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:3" ht="14.25" customHeight="1">
       <c r="C289" s="5"/>
     </row>
-    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:3" ht="14.25" customHeight="1">
       <c r="C290" s="5"/>
     </row>
-    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:3" ht="14.25" customHeight="1">
       <c r="C291" s="5"/>
     </row>
-    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:3" ht="14.25" customHeight="1">
       <c r="C292" s="5"/>
     </row>
-    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:3" ht="14.25" customHeight="1">
       <c r="C293" s="5"/>
     </row>
-    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:3" ht="14.25" customHeight="1">
       <c r="C294" s="5"/>
     </row>
-    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:3" ht="14.25" customHeight="1">
       <c r="C295" s="5"/>
     </row>
-    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:3" ht="14.25" customHeight="1">
       <c r="C296" s="5"/>
     </row>
-    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:3" ht="14.25" customHeight="1">
       <c r="C297" s="5"/>
     </row>
-    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:3" ht="14.25" customHeight="1">
       <c r="C298" s="5"/>
     </row>
-    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:3" ht="14.25" customHeight="1">
       <c r="C299" s="5"/>
     </row>
-    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:3" ht="14.25" customHeight="1">
       <c r="C300" s="5"/>
     </row>
-    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:3" ht="14.25" customHeight="1">
       <c r="C301" s="5"/>
     </row>
-    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="3:3" ht="14.25" customHeight="1">
       <c r="C302" s="5"/>
     </row>
-    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="3:3" ht="14.25" customHeight="1">
       <c r="C303" s="5"/>
     </row>
-    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="3:3" ht="14.25" customHeight="1">
       <c r="C304" s="5"/>
     </row>
-    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:3" ht="14.25" customHeight="1">
       <c r="C305" s="5"/>
     </row>
-    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:3" ht="14.25" customHeight="1">
       <c r="C306" s="5"/>
     </row>
-    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:3" ht="14.25" customHeight="1">
       <c r="C307" s="5"/>
     </row>
-    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:3" ht="14.25" customHeight="1">
       <c r="C308" s="5"/>
     </row>
-    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:3" ht="14.25" customHeight="1">
       <c r="C309" s="5"/>
     </row>
-    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:3" ht="14.25" customHeight="1">
       <c r="C310" s="5"/>
     </row>
-    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:3" ht="14.25" customHeight="1">
       <c r="C311" s="5"/>
     </row>
-    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:3" ht="14.25" customHeight="1">
       <c r="C312" s="5"/>
     </row>
-    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:3" ht="14.25" customHeight="1">
       <c r="C313" s="5"/>
     </row>
-    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:3" ht="14.25" customHeight="1">
       <c r="C314" s="5"/>
     </row>
-    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:3" ht="14.25" customHeight="1">
       <c r="C315" s="5"/>
     </row>
-    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:3" ht="14.25" customHeight="1">
       <c r="C316" s="5"/>
     </row>
-    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:3" ht="14.25" customHeight="1">
       <c r="C317" s="5"/>
     </row>
-    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="3:3" ht="14.25" customHeight="1">
       <c r="C318" s="5"/>
     </row>
-    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="3:3" ht="14.25" customHeight="1">
       <c r="C319" s="5"/>
     </row>
-    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="3:3" ht="14.25" customHeight="1">
       <c r="C320" s="5"/>
     </row>
-    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:3" ht="14.25" customHeight="1">
       <c r="C321" s="5"/>
     </row>
-    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:3" ht="14.25" customHeight="1">
       <c r="C322" s="5"/>
     </row>
-    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:3" ht="14.25" customHeight="1">
       <c r="C323" s="5"/>
     </row>
-    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:3" ht="14.25" customHeight="1">
       <c r="C324" s="5"/>
     </row>
-    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:3" ht="14.25" customHeight="1">
       <c r="C325" s="5"/>
     </row>
-    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:3" ht="14.25" customHeight="1">
       <c r="C326" s="5"/>
     </row>
-    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:3" ht="14.25" customHeight="1">
       <c r="C327" s="5"/>
     </row>
-    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:3" ht="14.25" customHeight="1">
       <c r="C328" s="5"/>
     </row>
-    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:3" ht="14.25" customHeight="1">
       <c r="C329" s="5"/>
     </row>
-    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:3" ht="14.25" customHeight="1">
       <c r="C330" s="5"/>
     </row>
-    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:3" ht="14.25" customHeight="1">
       <c r="C331" s="5"/>
     </row>
-    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:3" ht="14.25" customHeight="1">
       <c r="C332" s="5"/>
     </row>
-    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:3" ht="14.25" customHeight="1">
       <c r="C333" s="5"/>
     </row>
-    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="3:3" ht="14.25" customHeight="1">
       <c r="C334" s="5"/>
     </row>
-    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="3:3" ht="14.25" customHeight="1">
       <c r="C335" s="5"/>
     </row>
-    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="3:3" ht="14.25" customHeight="1">
       <c r="C336" s="5"/>
     </row>
-    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:3" ht="14.25" customHeight="1">
       <c r="C337" s="5"/>
     </row>
-    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:3" ht="14.25" customHeight="1">
       <c r="C338" s="5"/>
     </row>
-    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:3" ht="14.25" customHeight="1">
       <c r="C339" s="5"/>
     </row>
-    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:3" ht="14.25" customHeight="1">
       <c r="C340" s="5"/>
     </row>
-    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:3" ht="14.25" customHeight="1">
       <c r="C341" s="5"/>
     </row>
-    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:3" ht="14.25" customHeight="1">
       <c r="C342" s="5"/>
     </row>
-    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:3" ht="14.25" customHeight="1">
       <c r="C343" s="5"/>
     </row>
-    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:3" ht="14.25" customHeight="1">
       <c r="C344" s="5"/>
     </row>
-    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:3" ht="14.25" customHeight="1">
       <c r="C345" s="5"/>
     </row>
-    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:3" ht="14.25" customHeight="1">
       <c r="C346" s="5"/>
     </row>
-    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:3" ht="14.25" customHeight="1">
       <c r="C347" s="5"/>
     </row>
-    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:3" ht="14.25" customHeight="1">
       <c r="C348" s="5"/>
     </row>
-    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:3" ht="14.25" customHeight="1">
       <c r="C349" s="5"/>
     </row>
-    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="3:3" ht="14.25" customHeight="1">
       <c r="C350" s="5"/>
     </row>
-    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="3:3" ht="14.25" customHeight="1">
       <c r="C351" s="5"/>
     </row>
-    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="3:3" ht="14.25" customHeight="1">
       <c r="C352" s="5"/>
     </row>
-    <row r="353" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:3" ht="14.25" customHeight="1">
       <c r="C353" s="5"/>
     </row>
-    <row r="354" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:3" ht="14.25" customHeight="1">
       <c r="C354" s="5"/>
     </row>
-    <row r="355" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:3" ht="14.25" customHeight="1">
       <c r="C355" s="5"/>
     </row>
-    <row r="356" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C356" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D356" s="4">
-        <v>858943.22</v>
-      </c>
-      <c r="E356" s="7">
-        <v>8928.42</v>
-      </c>
-      <c r="F356" s="7">
-        <v>0</v>
-      </c>
-      <c r="G356" s="7">
-        <v>17833.34</v>
-      </c>
-      <c r="H356" s="7">
-        <v>5508.21</v>
-      </c>
-      <c r="I356" s="7">
-        <v>3076.9</v>
-      </c>
-      <c r="J356" s="7">
-        <v>369227</v>
-      </c>
-      <c r="K356" s="7">
-        <v>0</v>
-      </c>
-      <c r="L356" s="7">
-        <v>0</v>
-      </c>
-      <c r="M356" s="7">
-        <v>489716.22</v>
-      </c>
-    </row>
-    <row r="357" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C357" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D357" s="4">
-        <v>876776.56</v>
-      </c>
+    <row r="356" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C356" s="5"/>
+    </row>
+    <row r="357" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C357" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:L1048576">
+  <conditionalFormatting sqref="F1:M1048576">
     <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
+  <conditionalFormatting sqref="N1:N1048576">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>